<commit_message>
Updated FbaA proteomic value
</commit_message>
<xml_diff>
--- a/CME_ODE/model_data/proteomics.xlsx
+++ b/CME_ODE/model_data/proteomics.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidbianchi/test_pb/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zanert2/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2908,8 +2908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ431"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I40" workbookViewId="0">
-      <selection activeCell="X52" sqref="X52"/>
+    <sheetView tabSelected="1" topLeftCell="H43" workbookViewId="0">
+      <selection activeCell="O54" sqref="O54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7561,16 +7561,13 @@
         <v>3.4979687502515065E-3</v>
       </c>
       <c r="V57" s="3">
-        <f t="shared" si="6"/>
-        <v>227.15589353527665</v>
+        <v>775</v>
       </c>
       <c r="W57" s="3">
-        <f t="shared" si="7"/>
-        <v>250.47639897201407</v>
+        <v>775</v>
       </c>
       <c r="X57" s="3">
-        <f t="shared" si="8"/>
-        <v>269.44153689437303</v>
+        <v>775</v>
       </c>
     </row>
     <row r="58" spans="1:24" x14ac:dyDescent="0.2">
@@ -34903,7 +34900,7 @@
         <v>260115206.764624</v>
       </c>
       <c r="J387">
-        <f t="shared" ref="J387:J450" si="54">MEDIAN(G387:I387)</f>
+        <f t="shared" ref="J387:J430" si="54">MEDIAN(G387:I387)</f>
         <v>254944646.893958</v>
       </c>
       <c r="K387">
@@ -34916,7 +34913,7 @@
         <v>211403278.58344701</v>
       </c>
       <c r="N387">
-        <f t="shared" ref="N387:N450" si="55">MEDIAN(K387:M387)</f>
+        <f t="shared" ref="N387:N430" si="55">MEDIAN(K387:M387)</f>
         <v>180287999.29434901</v>
       </c>
       <c r="O387">
@@ -34929,7 +34926,7 @@
         <v>190430978.51916799</v>
       </c>
       <c r="R387">
-        <f t="shared" ref="R387:R450" si="56">MEDIAN(O387:Q387)</f>
+        <f t="shared" ref="R387:R430" si="56">MEDIAN(O387:Q387)</f>
         <v>193715073.445052</v>
       </c>
       <c r="S387">
@@ -38592,15 +38589,15 @@
       </c>
       <c r="V431">
         <f t="shared" si="63"/>
-        <v>77214.087973270216</v>
+        <v>77761.932079734921</v>
       </c>
       <c r="W431">
         <f t="shared" si="63"/>
-        <v>77214.927476256897</v>
+        <v>77739.451077284888</v>
       </c>
       <c r="X431">
         <f t="shared" si="63"/>
-        <v>77214.701800119918</v>
+        <v>77720.260263225558</v>
       </c>
     </row>
   </sheetData>

</xml_diff>